<commit_message>
finalised times and removed nas from final plot but not final leaderboards
</commit_message>
<xml_diff>
--- a/nn_jan.xlsx
+++ b/nn_jan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2135339w_student_gla_ac_uk/Documents/Projects/hs/nn_jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="11_9FF4AC7C9CB0901173FC1974DC7300627EEB5E2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B26C9813-74D9-4EE7-8676-11907491BC98}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_9FF4AC7C9CB0901173FC1974DC7300627EEB5E2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51BD23E6-2DDA-4623-B8F1-F3EC366F141D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="3">
-        <v>21.56</v>
+        <v>28.9</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="3">
-        <v>21.56</v>
+        <v>34.54</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>0</v>
@@ -513,7 +513,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="3">
-        <v>21.57</v>
+        <v>29.08</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>2</v>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="3">
-        <v>21.57</v>
+        <v>35.42</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>0</v>
@@ -554,7 +554,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="3">
-        <v>21.501000000000001</v>
+        <v>28.91</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>2</v>
@@ -562,9 +562,7 @@
       <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
-        <v>21.501000000000001</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
         <v>0</v>
       </c>
@@ -595,7 +593,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="3">
-        <v>22.041</v>
+        <v>29.2</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>2</v>
@@ -604,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="3">
-        <v>22.041</v>
+        <v>35.31</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>0</v>
@@ -636,20 +634,14 @@
       <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3">
-        <f>22.33/1.0165</f>
-        <v>21.967535661583867</v>
-      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="3">
-        <f>22.33/1.0165</f>
-        <v>21.967535661583867</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
         <v>0</v>
       </c>
@@ -680,7 +672,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="3">
-        <v>21.49</v>
+        <v>28.911000000000001</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>2</v>
@@ -689,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="3">
-        <v>21.49</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>0</v>
@@ -721,7 +713,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="3">
-        <v>21.5</v>
+        <v>28.89</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>2</v>
@@ -730,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="3">
-        <v>21.5</v>
+        <v>34.67</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>0</v>
@@ -761,9 +753,7 @@
       <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="3">
-        <v>21.73</v>
-      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
         <v>2</v>
       </c>
@@ -771,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="3">
-        <v>21.73</v>
+        <v>34.99</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>0</v>
@@ -803,7 +793,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="3">
-        <v>21.57</v>
+        <v>28.88</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>2</v>
@@ -812,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="3">
-        <v>21.57</v>
+        <v>35.21</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>0</v>
@@ -844,7 +834,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="3">
-        <v>21.6</v>
+        <v>29.07</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>2</v>
@@ -853,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="3">
-        <v>21.6</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>0</v>
@@ -885,7 +875,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="3">
-        <v>22.04</v>
+        <v>29.45</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>2</v>
@@ -894,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="3">
-        <v>22.04</v>
+        <v>36.409999999999997</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>0</v>
@@ -926,7 +916,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="3">
-        <v>21.89</v>
+        <v>29.37</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>2</v>
@@ -934,9 +924,7 @@
       <c r="H13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="3">
-        <v>21.89</v>
-      </c>
+      <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
         <v>0</v>
       </c>
@@ -967,7 +955,7 @@
         <v>22</v>
       </c>
       <c r="F14" s="3">
-        <v>21.62</v>
+        <v>28.98</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>2</v>
@@ -976,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="3">
-        <v>21.62</v>
+        <v>34.92</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>0</v>
@@ -1008,7 +996,7 @@
         <v>22</v>
       </c>
       <c r="F15" s="3">
-        <v>21.7</v>
+        <v>29.41</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>2</v>
@@ -1017,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="3">
-        <v>21.7</v>
+        <v>36.58</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>0</v>

</xml_diff>